<commit_message>
Se incluye hoja de datos para elementos de Analog Devices
//
</commit_message>
<xml_diff>
--- a/Lista de Elementos_16_05_2017/Lista_Luzbin.xlsx
+++ b/Lista de Elementos_16_05_2017/Lista_Luzbin.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Elementos totales" sheetId="2" r:id="rId2"/>
+    <sheet name="Luzbin" sheetId="1" r:id="rId1"/>
+    <sheet name="Elementos Digikey" sheetId="2" r:id="rId2"/>
+    <sheet name="Elementos Analog Devices" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Elementos totales'!$C$1:$K$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Elementos Analog Devices'!$C$1:$K$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Elementos Digikey'!$C$1:$J$42</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3337" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3381" uniqueCount="573">
   <si>
     <t>version</t>
   </si>
@@ -1693,6 +1695,63 @@
   </si>
   <si>
     <t>SOIC 8</t>
+  </si>
+  <si>
+    <t>Referencia</t>
+  </si>
+  <si>
+    <t>Precio 1</t>
+  </si>
+  <si>
+    <t>Precio 10</t>
+  </si>
+  <si>
+    <t>Precio 20</t>
+  </si>
+  <si>
+    <t>Precio 50</t>
+  </si>
+  <si>
+    <t>Precio 100</t>
+  </si>
+  <si>
+    <t>10 ld MSOP</t>
+  </si>
+  <si>
+    <t>AD9833SRMZ-EP-RL7</t>
+  </si>
+  <si>
+    <t>AD8421ARZ</t>
+  </si>
+  <si>
+    <t>8 ld SOIC</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>AD5270BRMZ-100</t>
+  </si>
+  <si>
+    <t>AD8651ARMZ</t>
+  </si>
+  <si>
+    <t>3 ld TO-92</t>
+  </si>
+  <si>
+    <t>ADR291GT9Z</t>
+  </si>
+  <si>
+    <t>8 ld MSOP</t>
+  </si>
+  <si>
+    <t>ADG819BRMZ</t>
+  </si>
+  <si>
+    <t>ADP3303ARZ-3.3</t>
   </si>
 </sst>
 </file>
@@ -2406,8 +2465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN579"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N4" workbookViewId="0">
-      <selection activeCell="Q58" sqref="Q58"/>
+    <sheetView topLeftCell="N70" workbookViewId="0">
+      <selection activeCell="P80" sqref="P80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,28 +2877,28 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R6" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="S6" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="T6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="U6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="V6" s="2" t="s">
         <v>201</v>
       </c>
       <c r="W6" s="1"/>
@@ -2873,28 +2932,28 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R7" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="S7" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="U7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="V7" s="2" t="s">
         <v>202</v>
       </c>
       <c r="W7" s="1"/>
@@ -2928,28 +2987,28 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R8" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="S8" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="T8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="U8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="V8" s="2" t="s">
         <v>203</v>
       </c>
       <c r="W8" s="1"/>
@@ -2983,28 +3042,28 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="R9" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="S9" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="T9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="U9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="V9" s="2" t="s">
         <v>204</v>
       </c>
       <c r="W9" s="1"/>
@@ -3038,28 +3097,28 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="N10" s="1"/>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="R10" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="S10" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="T10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="U10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="V10" s="2" t="s">
         <v>205</v>
       </c>
       <c r="W10" s="1"/>
@@ -3093,28 +3152,28 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="1" t="s">
+      <c r="O11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P11" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="R11" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="S11" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="T11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="U11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="V11" s="2" t="s">
         <v>206</v>
       </c>
       <c r="W11" s="1"/>
@@ -6417,31 +6476,31 @@
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
       <c r="N67" s="1"/>
-      <c r="O67" s="1" t="s">
+      <c r="O67" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="P67" s="1" t="s">
+      <c r="P67" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="Q67" s="1" t="s">
+      <c r="Q67" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="R67" s="1" t="s">
+      <c r="R67" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S67" s="1" t="s">
+      <c r="S67" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="T67" s="1" t="s">
+      <c r="T67" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U67" s="1" t="s">
+      <c r="U67" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="V67" s="1" t="s">
+      <c r="V67" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="W67" s="1" t="s">
+      <c r="W67" s="2" t="s">
         <v>505</v>
       </c>
       <c r="X67" s="1"/>
@@ -6535,31 +6594,31 @@
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="N69" s="1"/>
-      <c r="O69" s="1" t="s">
+      <c r="O69" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="P69" s="1" t="s">
+      <c r="P69" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="Q69" s="1" t="s">
+      <c r="Q69" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="R69" s="1" t="s">
+      <c r="R69" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S69" s="1" t="s">
+      <c r="S69" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="T69" s="1" t="s">
+      <c r="T69" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U69" s="1" t="s">
+      <c r="U69" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="V69" s="1" t="s">
+      <c r="V69" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="W69" s="1" t="s">
+      <c r="W69" s="2" t="s">
         <v>505</v>
       </c>
       <c r="X69" s="1"/>
@@ -7123,28 +7182,28 @@
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
       <c r="N79" s="1"/>
-      <c r="O79" s="1" t="s">
+      <c r="O79" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="P79" s="1" t="s">
+      <c r="P79" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="Q79" s="1" t="s">
+      <c r="Q79" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="R79" s="1" t="s">
+      <c r="R79" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S79" s="1" t="s">
+      <c r="S79" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="T79" s="1" t="s">
+      <c r="T79" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U79" s="1" t="s">
+      <c r="U79" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="V79" s="1" t="s">
+      <c r="V79" s="2" t="s">
         <v>274</v>
       </c>
       <c r="W79" s="1"/>
@@ -7178,28 +7237,28 @@
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
       <c r="N80" s="1"/>
-      <c r="O80" s="1" t="s">
+      <c r="O80" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="P80" s="1" t="s">
+      <c r="P80" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="Q80" s="1" t="s">
+      <c r="Q80" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="R80" s="1" t="s">
+      <c r="R80" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S80" s="1" t="s">
+      <c r="S80" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="T80" s="1" t="s">
+      <c r="T80" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U80" s="1" t="s">
+      <c r="U80" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="V80" s="1" t="s">
+      <c r="V80" s="2" t="s">
         <v>275</v>
       </c>
       <c r="W80" s="1"/>
@@ -32129,10 +32188,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K42"/>
+  <dimension ref="B1:O42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32144,10 +32203,9 @@
     <col min="7" max="7" width="8" style="16" customWidth="1"/>
     <col min="8" max="8" width="9" style="16" customWidth="1"/>
     <col min="9" max="9" width="8" style="16" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C1" s="5" t="s">
         <v>493</v>
       </c>
@@ -32173,10 +32231,22 @@
         <v>496</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+        <v>555</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C2" s="10" t="s">
         <v>362</v>
       </c>
@@ -32202,12 +32272,13 @@
         <f>G2+H2+I2</f>
         <v>4</v>
       </c>
-      <c r="K2" s="3">
-        <f>J2*5</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C3" s="10" t="s">
         <v>362</v>
       </c>
@@ -32233,12 +32304,13 @@
         <f t="shared" ref="J3:J42" si="0">G3+H3+I3</f>
         <v>32</v>
       </c>
-      <c r="K3" s="3">
-        <f t="shared" ref="K3:K42" si="1">J3*5</f>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C4" s="10" t="s">
         <v>362</v>
       </c>
@@ -32264,12 +32336,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K4" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C5" s="10" t="s">
         <v>363</v>
       </c>
@@ -32295,12 +32368,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K5" s="3">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
         <v>363</v>
       </c>
@@ -32326,12 +32400,13 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="K6" s="3">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C7" s="10" t="s">
         <v>362</v>
       </c>
@@ -32357,12 +32432,13 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="K7" s="3">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C8" s="10" t="s">
         <v>362</v>
       </c>
@@ -32388,12 +32464,13 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="K8" s="3">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C9" s="10" t="s">
         <v>363</v>
       </c>
@@ -32419,12 +32496,13 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K9" s="3">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C10" s="10" t="s">
         <v>362</v>
       </c>
@@ -32450,12 +32528,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="K10" s="3">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C11" s="10" t="s">
         <v>362</v>
       </c>
@@ -32481,12 +32560,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="K11" s="3">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C12" s="10" t="s">
         <v>511</v>
       </c>
@@ -32512,12 +32592,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K12" s="3">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C13" s="10" t="s">
         <v>511</v>
       </c>
@@ -32543,12 +32624,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K13" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C14" s="10" t="s">
         <v>516</v>
       </c>
@@ -32574,12 +32656,13 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="K14" s="3">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C15" s="10" t="s">
         <v>362</v>
       </c>
@@ -32605,12 +32688,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K15" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C16" s="10" t="s">
         <v>363</v>
       </c>
@@ -32636,12 +32720,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K16" s="3">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C17" s="10" t="s">
         <v>362</v>
       </c>
@@ -32667,12 +32752,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="K17" s="3">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C18" s="10" t="s">
         <v>526</v>
       </c>
@@ -32698,12 +32784,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K18" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C19" s="10" t="s">
         <v>526</v>
       </c>
@@ -32729,12 +32816,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K19" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C20" s="10" t="s">
         <v>363</v>
       </c>
@@ -32760,12 +32848,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K20" s="3">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C21" s="10" t="s">
         <v>363</v>
       </c>
@@ -32791,12 +32880,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K21" s="3">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C22" s="10" t="s">
         <v>363</v>
       </c>
@@ -32822,12 +32912,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K22" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C23" s="10" t="s">
         <v>363</v>
       </c>
@@ -32853,12 +32944,13 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="K23" s="3">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="17"/>
       <c r="C24" s="10" t="s">
         <v>363</v>
@@ -32885,12 +32977,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K24" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="17"/>
       <c r="C25" s="10" t="s">
         <v>362</v>
@@ -32917,12 +33010,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K25" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C26" s="10" t="s">
         <v>362</v>
       </c>
@@ -32948,12 +33042,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K26" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C27" s="10" t="s">
         <v>362</v>
       </c>
@@ -32979,12 +33074,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K27" s="3">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C28" s="10" t="s">
         <v>363</v>
       </c>
@@ -33010,12 +33106,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K28" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C29" s="10" t="s">
         <v>362</v>
       </c>
@@ -33041,12 +33138,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K29" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C30" s="10" t="s">
         <v>550</v>
       </c>
@@ -33072,12 +33170,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="K30" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C31" s="10"/>
       <c r="D31" s="18"/>
       <c r="E31" s="8"/>
@@ -33089,12 +33188,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K31" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C32" s="10"/>
       <c r="D32" s="18"/>
       <c r="E32" s="8"/>
@@ -33106,10 +33206,772 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K32" s="3">
-        <f t="shared" si="1"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C33" s="10"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="3">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C34" s="10"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C35" s="10"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C36" s="10"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C37" s="10"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C38" s="10"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C39" s="10"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C40" s="10"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C41" s="10"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C42" s="10"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="C1:J42"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C1:K42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C1" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C2" s="10" t="s">
+        <v>550</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>560</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="G2" s="12">
+        <v>0</v>
+      </c>
+      <c r="H2" s="12">
+        <v>0</v>
+      </c>
+      <c r="I2" s="12">
+        <v>2</v>
+      </c>
+      <c r="J2" s="3">
+        <f>G2+H2+I2</f>
+        <v>2</v>
+      </c>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C3" s="10" t="s">
+        <v>550</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>564</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>564</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>565</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J42" si="0">G3+H3+I3</f>
+        <v>2</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="10" t="s">
+        <v>550</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>560</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0</v>
+      </c>
+      <c r="I4" s="12">
+        <v>2</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="10" t="s">
+        <v>550</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0</v>
+      </c>
+      <c r="I5" s="12">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C6" s="10" t="s">
+        <v>550</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>568</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>569</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C7" s="10" t="s">
+        <v>550</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>570</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="G7" s="12">
+        <v>0</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0</v>
+      </c>
+      <c r="I7" s="12">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="10" t="s">
+        <v>550</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C9" s="10"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C10" s="10"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="10"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="10"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="10"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="10"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="10"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="10"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C17" s="10"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="10"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="10"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="10"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="10"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="10"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="10"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="10"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="10"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="10"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="10"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C28" s="10"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C29" s="10"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="10"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C31" s="10"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C32" s="10"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="3"/>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C33" s="10"/>
@@ -33123,10 +33985,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K33" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="K33" s="3"/>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C34" s="10"/>
@@ -33140,10 +33999,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K34" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="K34" s="3"/>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C35" s="10"/>
@@ -33157,10 +34013,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K35" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="K35" s="3"/>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C36" s="10"/>
@@ -33174,10 +34027,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K36" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="K36" s="3"/>
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C37" s="10"/>
@@ -33191,10 +34041,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K37" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="K37" s="3"/>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C38" s="10"/>
@@ -33208,10 +34055,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K38" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="K38" s="3"/>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C39" s="10"/>
@@ -33225,10 +34069,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K39" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="K39" s="3"/>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C40" s="10"/>
@@ -33242,10 +34083,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K40" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="K40" s="3"/>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C41" s="10"/>
@@ -33259,10 +34097,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K41" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="K41" s="3"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C42" s="10"/>
@@ -33276,10 +34111,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K42" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="K42" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="C1:K42"/>

</xml_diff>